<commit_message>
updated keys: run 7 and misc. notes
</commit_message>
<xml_diff>
--- a/Experiment Key.xlsx
+++ b/Experiment Key.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DrCoffey\Documents\GitHub\CoffeyBehavior\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Todd Appleby\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C9CEA4-4A41-4C28-9578-2545E9C92440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CB8E6B-8550-4165-82DC-B02BEAA9DA45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19080" windowHeight="17400" xr2:uid="{CD7F1C8E-C617-4CB6-9DA2-6C0677DD65A5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CD7F1C8E-C617-4CB6-9DA2-6C0677DD65A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="16">
   <si>
     <t>Run</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Extinction2</t>
+  </si>
+  <si>
+    <t>SA</t>
   </si>
 </sst>
 </file>
@@ -216,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -266,16 +269,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -480,8 +474,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{66D5D3F3-56B7-46A6-A496-8A38EB2958B8}" name="Table1" displayName="Table1" ref="A1:G175" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7">
-  <autoFilter ref="A1:G175" xr:uid="{66D5D3F3-56B7-46A6-A496-8A38EB2958B8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{66D5D3F3-56B7-46A6-A496-8A38EB2958B8}" name="Table1" displayName="Table1" ref="A1:G190" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7">
+  <autoFilter ref="A1:G190" xr:uid="{66D5D3F3-56B7-46A6-A496-8A38EB2958B8}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G144">
     <sortCondition ref="A1:A144"/>
   </sortState>
@@ -815,11 +809,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB0A6A4-2587-470F-932D-101544863E20}">
-  <dimension ref="A1:G175"/>
+  <dimension ref="A1:G190"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A136" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C133" sqref="C133"/>
+      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G176" sqref="G176:G190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2494,25 +2488,25 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="18">
-        <v>4</v>
-      </c>
-      <c r="B73" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C73" s="19">
+      <c r="A73" s="1">
+        <v>4</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" s="11">
         <v>45593</v>
       </c>
-      <c r="D73" s="18">
-        <v>6</v>
-      </c>
-      <c r="E73" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F73" s="18">
-        <v>70</v>
-      </c>
-      <c r="G73" s="18">
+      <c r="D73" s="1">
+        <v>6</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F73" s="1">
+        <v>70</v>
+      </c>
+      <c r="G73" s="1">
         <v>1.9310000000000001E-2</v>
       </c>
     </row>
@@ -3000,25 +2994,25 @@
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="18">
-        <v>4</v>
-      </c>
-      <c r="B95" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C95" s="20">
+      <c r="A95" s="1">
+        <v>4</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C95" s="10">
         <v>45587</v>
       </c>
-      <c r="D95" s="18">
+      <c r="D95" s="1">
         <v>2</v>
       </c>
-      <c r="E95" s="18" t="s">
+      <c r="E95" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F95" s="18">
-        <v>70</v>
-      </c>
-      <c r="G95" s="18">
+      <c r="F95" s="1">
+        <v>70</v>
+      </c>
+      <c r="G95" s="1">
         <v>1.9310000000000001E-2</v>
       </c>
     </row>
@@ -3989,7 +3983,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A138" s="15">
+      <c r="A138" s="7">
         <v>5</v>
       </c>
       <c r="B138" s="1" t="s">
@@ -4012,19 +4006,19 @@
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A139" s="15">
+      <c r="A139" s="7">
         <v>5</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C139" s="17">
+      <c r="C139" s="10">
         <v>45733</v>
       </c>
       <c r="D139" s="1">
         <v>26</v>
       </c>
-      <c r="E139" s="16" t="s">
+      <c r="E139" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F139" s="1">
@@ -4035,19 +4029,19 @@
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A140" s="15">
+      <c r="A140" s="7">
         <v>5</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C140" s="17">
+      <c r="C140" s="10">
         <v>45734</v>
       </c>
       <c r="D140" s="1">
         <v>27</v>
       </c>
-      <c r="E140" s="16" t="s">
+      <c r="E140" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F140" s="1">
@@ -4058,19 +4052,19 @@
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A141" s="15">
+      <c r="A141" s="7">
         <v>5</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C141" s="17">
+      <c r="C141" s="10">
         <v>45735</v>
       </c>
       <c r="D141" s="1">
         <v>28</v>
       </c>
-      <c r="E141" s="16" t="s">
+      <c r="E141" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F141" s="1">
@@ -4081,19 +4075,19 @@
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A142" s="15">
+      <c r="A142" s="7">
         <v>5</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C142" s="17">
+      <c r="C142" s="10">
         <v>45736</v>
       </c>
       <c r="D142" s="1">
         <v>29</v>
       </c>
-      <c r="E142" s="16" t="s">
+      <c r="E142" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F142" s="1">
@@ -4104,19 +4098,19 @@
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A143" s="15">
+      <c r="A143" s="7">
         <v>5</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C143" s="17">
+      <c r="C143" s="10">
         <v>45737</v>
       </c>
       <c r="D143" s="1">
         <v>30</v>
       </c>
-      <c r="E143" s="16" t="s">
+      <c r="E143" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F143" s="1">
@@ -4860,6 +4854,351 @@
       </c>
       <c r="G175" s="8">
         <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A176" s="15">
+        <v>7</v>
+      </c>
+      <c r="B176" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C176" s="17">
+        <v>45790</v>
+      </c>
+      <c r="D176" s="16">
+        <v>1</v>
+      </c>
+      <c r="E176" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F176" s="16">
+        <v>70</v>
+      </c>
+      <c r="G176" s="8">
+        <v>1.9310000000000001E-2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A177" s="15">
+        <v>7</v>
+      </c>
+      <c r="B177" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C177" s="17">
+        <v>45791</v>
+      </c>
+      <c r="D177" s="16">
+        <v>2</v>
+      </c>
+      <c r="E177" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F177" s="16">
+        <v>70</v>
+      </c>
+      <c r="G177" s="8">
+        <v>1.9310000000000001E-2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A178" s="15">
+        <v>7</v>
+      </c>
+      <c r="B178" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C178" s="17">
+        <v>45792</v>
+      </c>
+      <c r="D178" s="16">
+        <v>3</v>
+      </c>
+      <c r="E178" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F178" s="16">
+        <v>70</v>
+      </c>
+      <c r="G178" s="8">
+        <v>1.9310000000000001E-2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A179" s="15">
+        <v>7</v>
+      </c>
+      <c r="B179" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C179" s="17">
+        <v>45793</v>
+      </c>
+      <c r="D179" s="16">
+        <v>4</v>
+      </c>
+      <c r="E179" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F179" s="16">
+        <v>70</v>
+      </c>
+      <c r="G179" s="8">
+        <v>1.9310000000000001E-2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A180" s="15">
+        <v>7</v>
+      </c>
+      <c r="B180" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C180" s="17">
+        <v>45794</v>
+      </c>
+      <c r="D180" s="16">
+        <v>5</v>
+      </c>
+      <c r="E180" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F180" s="16">
+        <v>70</v>
+      </c>
+      <c r="G180" s="8">
+        <v>1.9310000000000001E-2</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A181" s="15">
+        <v>7</v>
+      </c>
+      <c r="B181" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C181" s="17">
+        <v>45797</v>
+      </c>
+      <c r="D181" s="16">
+        <v>6</v>
+      </c>
+      <c r="E181" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F181" s="16">
+        <v>70</v>
+      </c>
+      <c r="G181" s="8">
+        <v>1.9310000000000001E-2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A182" s="15">
+        <v>7</v>
+      </c>
+      <c r="B182" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C182" s="17">
+        <v>45798</v>
+      </c>
+      <c r="D182" s="16">
+        <v>7</v>
+      </c>
+      <c r="E182" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F182" s="16">
+        <v>70</v>
+      </c>
+      <c r="G182" s="8">
+        <v>1.9310000000000001E-2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A183" s="15">
+        <v>7</v>
+      </c>
+      <c r="B183" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C183" s="17">
+        <v>45799</v>
+      </c>
+      <c r="D183" s="16">
+        <v>8</v>
+      </c>
+      <c r="E183" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F183" s="16">
+        <v>70</v>
+      </c>
+      <c r="G183" s="8">
+        <v>1.9310000000000001E-2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A184" s="15">
+        <v>7</v>
+      </c>
+      <c r="B184" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C184" s="17">
+        <v>45800</v>
+      </c>
+      <c r="D184" s="16">
+        <v>9</v>
+      </c>
+      <c r="E184" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F184" s="16">
+        <v>70</v>
+      </c>
+      <c r="G184" s="8">
+        <v>1.9310000000000001E-2</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A185" s="15">
+        <v>7</v>
+      </c>
+      <c r="B185" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C185" s="17">
+        <v>45801</v>
+      </c>
+      <c r="D185" s="16">
+        <v>10</v>
+      </c>
+      <c r="E185" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F185" s="16">
+        <v>70</v>
+      </c>
+      <c r="G185" s="8">
+        <v>1.9310000000000001E-2</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A186" s="15">
+        <v>7</v>
+      </c>
+      <c r="B186" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C186" s="17">
+        <v>45804</v>
+      </c>
+      <c r="D186" s="16">
+        <v>11</v>
+      </c>
+      <c r="E186" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F186" s="16">
+        <v>70</v>
+      </c>
+      <c r="G186" s="8">
+        <v>1.9310000000000001E-2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A187" s="15">
+        <v>7</v>
+      </c>
+      <c r="B187" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C187" s="17">
+        <v>45805</v>
+      </c>
+      <c r="D187" s="16">
+        <v>12</v>
+      </c>
+      <c r="E187" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F187" s="16">
+        <v>70</v>
+      </c>
+      <c r="G187" s="8">
+        <v>1.9310000000000001E-2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A188" s="15">
+        <v>7</v>
+      </c>
+      <c r="B188" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C188" s="17">
+        <v>45806</v>
+      </c>
+      <c r="D188" s="16">
+        <v>13</v>
+      </c>
+      <c r="E188" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F188" s="16">
+        <v>70</v>
+      </c>
+      <c r="G188" s="8">
+        <v>1.9310000000000001E-2</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A189" s="15">
+        <v>7</v>
+      </c>
+      <c r="B189" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C189" s="17">
+        <v>45807</v>
+      </c>
+      <c r="D189" s="16">
+        <v>14</v>
+      </c>
+      <c r="E189" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F189" s="16">
+        <v>70</v>
+      </c>
+      <c r="G189" s="8">
+        <v>1.9310000000000001E-2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A190" s="15">
+        <v>7</v>
+      </c>
+      <c r="B190" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C190" s="17">
+        <v>45808</v>
+      </c>
+      <c r="D190" s="16">
+        <v>15</v>
+      </c>
+      <c r="E190" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F190" s="16">
+        <v>70</v>
+      </c>
+      <c r="G190" s="8">
+        <v>1.9310000000000001E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>